<commit_message>
stored country name in array
</commit_message>
<xml_diff>
--- a/Human_Development_Index.xlsx
+++ b/Human_Development_Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thong\ImpactHack2020\interactive_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55EB846-1E9F-4CF4-849C-D67EB033C41F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B497244-7F57-4086-9A19-D18EE231C8F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="408">
   <si>
     <t>Human development index (HDI)</t>
   </si>
@@ -593,6 +593,60 @@
   </si>
   <si>
     <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>Human Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Very high human development</t>
+  </si>
+  <si>
+    <t>High human development</t>
+  </si>
+  <si>
+    <t>Medium human development</t>
+  </si>
+  <si>
+    <t>Low human development</t>
+  </si>
+  <si>
+    <t>Developing Countries</t>
+  </si>
+  <si>
+    <t>Regions</t>
+  </si>
+  <si>
+    <t>Arab States</t>
+  </si>
+  <si>
+    <t>East Asia and the Pacific</t>
+  </si>
+  <si>
+    <t>Europe and Central Asia</t>
+  </si>
+  <si>
+    <t>Latin America and the Caribbean</t>
+  </si>
+  <si>
+    <t>South Asia</t>
+  </si>
+  <si>
+    <t>Sub-Saharan Africa</t>
+  </si>
+  <si>
+    <t>Least Developed Countries</t>
+  </si>
+  <si>
+    <t>Small Island Developing States</t>
+  </si>
+  <si>
+    <t>Organization for Economic Co-operation and Development</t>
+  </si>
+  <si>
+    <t>World</t>
   </si>
   <si>
     <t>AF</t>
@@ -2040,10 +2094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF197"/>
+  <dimension ref="A1:AF214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,7 +2118,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
       <c r="D2">
         <v>1990</v>
@@ -2162,7 +2216,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="D3">
         <v>0.29799999999999999</v>
@@ -2260,7 +2314,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>192</v>
+        <v>210</v>
       </c>
       <c r="D4">
         <v>0.64400000000000002</v>
@@ -2358,7 +2412,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
       <c r="D5">
         <v>0.57799999999999996</v>
@@ -2456,7 +2510,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -2554,7 +2608,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -2652,7 +2706,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -2750,7 +2804,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="D9">
         <v>0.70699999999999996</v>
@@ -2848,7 +2902,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="D10">
         <v>0.63300000000000001</v>
@@ -2946,7 +3000,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="D11">
         <v>0.86599999999999999</v>
@@ -3044,7 +3098,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="D12">
         <v>0.79500000000000004</v>
@@ -3142,7 +3196,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -3240,7 +3294,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -3338,7 +3392,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="D15">
         <v>0.73599999999999999</v>
@@ -3436,7 +3490,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>207</v>
+        <v>225</v>
       </c>
       <c r="D16">
         <v>0.38800000000000001</v>
@@ -3534,7 +3588,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
       <c r="D17">
         <v>0.73199999999999998</v>
@@ -3632,7 +3686,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -3730,7 +3784,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="D19">
         <v>0.80600000000000005</v>
@@ -3828,7 +3882,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="D20">
         <v>0.61299999999999999</v>
@@ -3926,7 +3980,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>214</v>
+        <v>232</v>
       </c>
       <c r="D21">
         <v>0.34799999999999998</v>
@@ -4024,7 +4078,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
@@ -4119,10 +4173,10 @@
         <v>114</v>
       </c>
       <c r="B23" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="D23">
         <v>0.54</v>
@@ -4220,7 +4274,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -4318,7 +4372,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="D25">
         <v>0.56999999999999995</v>
@@ -4416,7 +4470,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="D26">
         <v>0.61299999999999999</v>
@@ -4514,7 +4568,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="D27">
         <v>0.76800000000000002</v>
@@ -4612,7 +4666,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="D28">
         <v>0.69399999999999995</v>
@@ -4710,7 +4764,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -4808,7 +4862,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="D30">
         <v>0.29499999999999998</v>
@@ -5004,7 +5058,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="D32">
         <v>0.38400000000000001</v>
@@ -5102,7 +5156,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="D33">
         <v>0.44500000000000001</v>
@@ -5200,7 +5254,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="D34">
         <v>0.85</v>
@@ -5298,7 +5352,7 @@
         <v>35</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="D35">
         <v>0.32</v>
@@ -5396,7 +5450,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -5494,7 +5548,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="D37">
         <v>0.70299999999999996</v>
@@ -5592,7 +5646,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="D38">
         <v>0.501</v>
@@ -5690,7 +5744,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="D39">
         <v>0.6</v>
@@ -5788,7 +5842,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -5886,7 +5940,7 @@
         <v>41</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="D41">
         <v>0.53100000000000003</v>
@@ -5981,10 +6035,10 @@
         <v>179</v>
       </c>
       <c r="B42" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>222</v>
+        <v>240</v>
       </c>
       <c r="D42">
         <v>0.377</v>
@@ -6082,7 +6136,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="D43">
         <v>0.65500000000000003</v>
@@ -6180,7 +6234,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="D44">
         <v>0.67</v>
@@ -6278,7 +6332,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="D45">
         <v>0.67600000000000005</v>
@@ -6376,7 +6430,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="D46">
         <v>0.73099999999999998</v>
@@ -6572,7 +6626,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="D48">
         <v>0.39100000000000001</v>
@@ -6670,7 +6724,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>241</v>
+        <v>259</v>
       </c>
       <c r="D49">
         <v>0.79900000000000004</v>
@@ -6768,7 +6822,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
@@ -6866,7 +6920,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -6964,7 +7018,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="D52">
         <v>0.59299999999999997</v>
@@ -7062,7 +7116,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="D53">
         <v>0.64200000000000002</v>
@@ -7160,7 +7214,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="D54">
         <v>0.54600000000000004</v>
@@ -7258,7 +7312,7 @@
         <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="D55">
         <v>0.52900000000000003</v>
@@ -7356,7 +7410,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
@@ -7454,7 +7508,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -7552,7 +7606,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="D58">
         <v>0.73</v>
@@ -7748,7 +7802,7 @@
         <v>59</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -7846,7 +7900,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="D61">
         <v>0.64</v>
@@ -7944,7 +7998,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="D62">
         <v>0.78400000000000003</v>
@@ -8042,7 +8096,7 @@
         <v>62</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="D63">
         <v>0.78</v>
@@ -8140,7 +8194,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="D64">
         <v>0.61899999999999999</v>
@@ -8238,7 +8292,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="D65">
         <v>0.32800000000000001</v>
@@ -8336,7 +8390,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -8434,7 +8488,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="D67">
         <v>0.80100000000000005</v>
@@ -8532,7 +8586,7 @@
         <v>67</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>285</v>
+        <v>303</v>
       </c>
       <c r="D68">
         <v>0.45400000000000001</v>
@@ -8630,7 +8684,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="D69">
         <v>0.753</v>
@@ -8728,7 +8782,7 @@
         <v>69</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
@@ -8826,7 +8880,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="D71">
         <v>0.47699999999999998</v>
@@ -8924,7 +8978,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="D72">
         <v>0.27800000000000002</v>
@@ -9022,7 +9076,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
@@ -9120,7 +9174,7 @@
         <v>73</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="D74">
         <v>0.53700000000000003</v>
@@ -9218,7 +9272,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="D75">
         <v>0.41199999999999998</v>
@@ -9316,7 +9370,7 @@
         <v>75</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="D76">
         <v>0.50800000000000001</v>
@@ -9512,7 +9566,7 @@
         <v>77</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="D78">
         <v>0.70399999999999996</v>
@@ -9610,7 +9664,7 @@
         <v>78</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="D79">
         <v>0.80400000000000005</v>
@@ -9708,7 +9762,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="D80">
         <v>0.43099999999999999</v>
@@ -9806,7 +9860,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="D81">
         <v>0.52500000000000002</v>
@@ -9901,10 +9955,10 @@
         <v>65</v>
       </c>
       <c r="B82" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="D82">
         <v>0.57699999999999996</v>
@@ -10002,7 +10056,7 @@
         <v>81</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="D83">
         <v>0.57399999999999995</v>
@@ -10100,7 +10154,7 @@
         <v>82</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="D84">
         <v>0.76400000000000001</v>
@@ -10198,7 +10252,7 @@
         <v>83</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="D85">
         <v>0.79200000000000004</v>
@@ -10296,7 +10350,7 @@
         <v>84</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="D86">
         <v>0.76900000000000002</v>
@@ -10394,7 +10448,7 @@
         <v>85</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="D87">
         <v>0.64100000000000001</v>
@@ -10492,7 +10546,7 @@
         <v>86</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
       <c r="D88">
         <v>0.81599999999999995</v>
@@ -10590,7 +10644,7 @@
         <v>87</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="D89">
         <v>0.61599999999999999</v>
@@ -10688,7 +10742,7 @@
         <v>88</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
       <c r="D90">
         <v>0.69</v>
@@ -10786,7 +10840,7 @@
         <v>89</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="D91">
         <v>0.46700000000000003</v>
@@ -10884,7 +10938,7 @@
         <v>90</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>307</v>
+        <v>325</v>
       </c>
       <c r="D92" t="s">
         <v>7</v>
@@ -10982,7 +11036,7 @@
         <v>91</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="D93">
         <v>0.72799999999999998</v>
@@ -11080,7 +11134,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>308</v>
+        <v>326</v>
       </c>
       <c r="D94">
         <v>0.71199999999999997</v>
@@ -11178,7 +11232,7 @@
         <v>93</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="D95">
         <v>0.61799999999999999</v>
@@ -11276,7 +11330,7 @@
         <v>94</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="D96">
         <v>0.39900000000000002</v>
@@ -11374,7 +11428,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>310</v>
+        <v>328</v>
       </c>
       <c r="D97">
         <v>0.69799999999999995</v>
@@ -11472,7 +11526,7 @@
         <v>96</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>311</v>
+        <v>329</v>
       </c>
       <c r="D98" t="s">
         <v>7</v>
@@ -11570,7 +11624,7 @@
         <v>97</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>312</v>
+        <v>330</v>
       </c>
       <c r="D99">
         <v>0.48799999999999999</v>
@@ -11668,7 +11722,7 @@
         <v>98</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>313</v>
+        <v>331</v>
       </c>
       <c r="D100" t="s">
         <v>7</v>
@@ -11766,7 +11820,7 @@
         <v>99</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>314</v>
+        <v>332</v>
       </c>
       <c r="D101">
         <v>0.67600000000000005</v>
@@ -11864,7 +11918,7 @@
         <v>100</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="D102" t="s">
         <v>7</v>
@@ -11962,7 +12016,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="D103">
         <v>0.73199999999999998</v>
@@ -12060,7 +12114,7 @@
         <v>102</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
       <c r="D104">
         <v>0.79100000000000004</v>
@@ -12158,7 +12212,7 @@
         <v>103</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="D105" t="s">
         <v>7</v>
@@ -12256,7 +12310,7 @@
         <v>104</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>317</v>
+        <v>335</v>
       </c>
       <c r="D106">
         <v>0.30299999999999999</v>
@@ -12354,7 +12408,7 @@
         <v>105</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>318</v>
+        <v>336</v>
       </c>
       <c r="D107">
         <v>0.64400000000000002</v>
@@ -12452,7 +12506,7 @@
         <v>106</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>319</v>
+        <v>337</v>
       </c>
       <c r="D108" t="s">
         <v>7</v>
@@ -12550,7 +12604,7 @@
         <v>107</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>320</v>
+        <v>338</v>
       </c>
       <c r="D109">
         <v>0.23100000000000001</v>
@@ -12648,7 +12702,7 @@
         <v>108</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>321</v>
+        <v>339</v>
       </c>
       <c r="D110">
         <v>0.74399999999999999</v>
@@ -12746,7 +12800,7 @@
         <v>109</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>322</v>
+        <v>340</v>
       </c>
       <c r="D111" t="s">
         <v>7</v>
@@ -12844,7 +12898,7 @@
         <v>110</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="D112">
         <v>0.378</v>
@@ -12942,7 +12996,7 @@
         <v>111</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>323</v>
+        <v>341</v>
       </c>
       <c r="D113">
         <v>0.62</v>
@@ -13040,7 +13094,7 @@
         <v>112</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="D114">
         <v>0.65200000000000002</v>
@@ -13135,10 +13189,10 @@
         <v>135</v>
       </c>
       <c r="B115" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>326</v>
+        <v>344</v>
       </c>
       <c r="D115" t="s">
         <v>7</v>
@@ -13233,10 +13287,10 @@
         <v>107</v>
       </c>
       <c r="B116" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>328</v>
+        <v>346</v>
       </c>
       <c r="D116">
         <v>0.65300000000000002</v>
@@ -13334,7 +13388,7 @@
         <v>113</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>329</v>
+        <v>347</v>
       </c>
       <c r="D117">
         <v>0.58299999999999996</v>
@@ -13432,7 +13486,7 @@
         <v>114</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="D118" t="s">
         <v>7</v>
@@ -13530,7 +13584,7 @@
         <v>115</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="D119">
         <v>0.45800000000000002</v>
@@ -13628,7 +13682,7 @@
         <v>116</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>330</v>
+        <v>348</v>
       </c>
       <c r="D120">
         <v>0.217</v>
@@ -13726,7 +13780,7 @@
         <v>117</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="D121">
         <v>0.35</v>
@@ -13824,7 +13878,7 @@
         <v>118</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
       <c r="D122">
         <v>0.57899999999999996</v>
@@ -13922,7 +13976,7 @@
         <v>119</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>331</v>
+        <v>349</v>
       </c>
       <c r="D123">
         <v>0.38</v>
@@ -14020,7 +14074,7 @@
         <v>120</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="D124">
         <v>0.83</v>
@@ -14118,7 +14172,7 @@
         <v>121</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>333</v>
+        <v>351</v>
       </c>
       <c r="D125">
         <v>0.82</v>
@@ -14216,7 +14270,7 @@
         <v>122</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="D126">
         <v>0.49399999999999999</v>
@@ -14314,7 +14368,7 @@
         <v>123</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="D127">
         <v>0.21299999999999999</v>
@@ -14412,7 +14466,7 @@
         <v>124</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>332</v>
+        <v>350</v>
       </c>
       <c r="D128" t="s">
         <v>7</v>
@@ -14510,7 +14564,7 @@
         <v>125</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>334</v>
+        <v>352</v>
       </c>
       <c r="D129" t="s">
         <v>7</v>
@@ -14608,7 +14662,7 @@
         <v>126</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>335</v>
+        <v>353</v>
       </c>
       <c r="D130">
         <v>0.85</v>
@@ -14706,7 +14760,7 @@
         <v>127</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>336</v>
+        <v>354</v>
       </c>
       <c r="D131" t="s">
         <v>7</v>
@@ -14804,7 +14858,7 @@
         <v>128</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>337</v>
+        <v>355</v>
       </c>
       <c r="D132">
         <v>0.40400000000000003</v>
@@ -14902,7 +14956,7 @@
         <v>129</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>338</v>
+        <v>356</v>
       </c>
       <c r="D133" t="s">
         <v>7</v>
@@ -15000,7 +15054,7 @@
         <v>130</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>339</v>
+        <v>357</v>
       </c>
       <c r="D134" t="s">
         <v>7</v>
@@ -15098,7 +15152,7 @@
         <v>131</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="D135">
         <v>0.65900000000000003</v>
@@ -15196,7 +15250,7 @@
         <v>132</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
       <c r="D136">
         <v>0.377</v>
@@ -15294,7 +15348,7 @@
         <v>133</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>341</v>
+        <v>359</v>
       </c>
       <c r="D137">
         <v>0.58799999999999997</v>
@@ -15392,7 +15446,7 @@
         <v>134</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>342</v>
+        <v>360</v>
       </c>
       <c r="D138">
         <v>0.61299999999999999</v>
@@ -15490,7 +15544,7 @@
         <v>135</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>343</v>
+        <v>361</v>
       </c>
       <c r="D139">
         <v>0.59</v>
@@ -15588,7 +15642,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>344</v>
+        <v>362</v>
       </c>
       <c r="D140">
         <v>0.71199999999999997</v>
@@ -15686,7 +15740,7 @@
         <v>137</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>345</v>
+        <v>363</v>
       </c>
       <c r="D141">
         <v>0.71099999999999997</v>
@@ -15784,7 +15838,7 @@
         <v>138</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="D142">
         <v>0.75700000000000001</v>
@@ -15882,7 +15936,7 @@
         <v>139</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>347</v>
+        <v>365</v>
       </c>
       <c r="D143">
         <v>0.70099999999999996</v>
@@ -15980,7 +16034,7 @@
         <v>140</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>348</v>
+        <v>366</v>
       </c>
       <c r="D144">
         <v>0.73399999999999999</v>
@@ -16078,7 +16132,7 @@
         <v>141</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>349</v>
+        <v>367</v>
       </c>
       <c r="D145">
         <v>0.245</v>
@@ -16176,7 +16230,7 @@
         <v>142</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>350</v>
+        <v>368</v>
       </c>
       <c r="D146" t="s">
         <v>7</v>
@@ -16274,7 +16328,7 @@
         <v>143</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>351</v>
+        <v>369</v>
       </c>
       <c r="D147" t="s">
         <v>7</v>
@@ -16372,7 +16426,7 @@
         <v>144</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>352</v>
+        <v>370</v>
       </c>
       <c r="D148" t="s">
         <v>7</v>
@@ -16470,7 +16524,7 @@
         <v>145</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>353</v>
+        <v>371</v>
       </c>
       <c r="D149">
         <v>0.621</v>
@@ -16568,7 +16622,7 @@
         <v>146</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="D150">
         <v>0.437</v>
@@ -16666,7 +16720,7 @@
         <v>147</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="D151">
         <v>0.69799999999999995</v>
@@ -16764,7 +16818,7 @@
         <v>148</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>271</v>
+        <v>289</v>
       </c>
       <c r="D152">
         <v>0.377</v>
@@ -16862,7 +16916,7 @@
         <v>149</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>355</v>
+        <v>373</v>
       </c>
       <c r="D153">
         <v>0.70599999999999996</v>
@@ -16960,7 +17014,7 @@
         <v>150</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="D154" t="s">
         <v>7</v>
@@ -17058,7 +17112,7 @@
         <v>151</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="D155">
         <v>0.27</v>
@@ -17156,7 +17210,7 @@
         <v>152</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>357</v>
+        <v>375</v>
       </c>
       <c r="D156">
         <v>0.71799999999999997</v>
@@ -17254,7 +17308,7 @@
         <v>153</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>358</v>
+        <v>376</v>
       </c>
       <c r="D157">
         <v>0.73899999999999999</v>
@@ -17352,7 +17406,7 @@
         <v>154</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>359</v>
+        <v>377</v>
       </c>
       <c r="D158">
         <v>0.82899999999999996</v>
@@ -17450,7 +17504,7 @@
         <v>155</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>360</v>
+        <v>378</v>
       </c>
       <c r="D159" t="s">
         <v>7</v>
@@ -17548,7 +17602,7 @@
         <v>156</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>363</v>
+        <v>381</v>
       </c>
       <c r="D160">
         <v>0.625</v>
@@ -17646,7 +17700,7 @@
         <v>157</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="D161" t="s">
         <v>7</v>
@@ -17744,7 +17798,7 @@
         <v>158</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="D162">
         <v>0.754</v>
@@ -17842,7 +17896,7 @@
         <v>159</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>364</v>
+        <v>382</v>
       </c>
       <c r="D163">
         <v>0.625</v>
@@ -17940,7 +17994,7 @@
         <v>160</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>365</v>
+        <v>383</v>
       </c>
       <c r="D164">
         <v>0.33200000000000002</v>
@@ -18038,7 +18092,7 @@
         <v>161</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="D165" t="s">
         <v>7</v>
@@ -18136,7 +18190,7 @@
         <v>162</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>361</v>
+        <v>379</v>
       </c>
       <c r="D166">
         <v>0.81599999999999995</v>
@@ -18234,7 +18288,7 @@
         <v>163</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>212</v>
+        <v>230</v>
       </c>
       <c r="D167">
         <v>0.83199999999999996</v>
@@ -18332,7 +18386,7 @@
         <v>164</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>366</v>
+        <v>384</v>
       </c>
       <c r="D168">
         <v>0.55800000000000005</v>
@@ -18430,7 +18484,7 @@
         <v>165</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>367</v>
+        <v>385</v>
       </c>
       <c r="D169">
         <v>0.60299999999999998</v>
@@ -18525,10 +18579,10 @@
         <v>159</v>
       </c>
       <c r="B170" t="s">
-        <v>368</v>
+        <v>386</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>369</v>
+        <v>387</v>
       </c>
       <c r="D170">
         <v>0.373</v>
@@ -18626,7 +18680,7 @@
         <v>166</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>374</v>
+        <v>392</v>
       </c>
       <c r="D171">
         <v>0.57399999999999995</v>
@@ -18724,7 +18778,7 @@
         <v>167</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>377</v>
+        <v>395</v>
       </c>
       <c r="D172" t="s">
         <v>7</v>
@@ -18822,7 +18876,7 @@
         <v>168</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>362</v>
+        <v>380</v>
       </c>
       <c r="D173">
         <v>0.40500000000000003</v>
@@ -18920,7 +18974,7 @@
         <v>169</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
       <c r="D174">
         <v>0.64500000000000002</v>
@@ -19018,7 +19072,7 @@
         <v>170</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="D175">
         <v>0.66700000000000004</v>
@@ -19116,7 +19170,7 @@
         <v>171</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="D176">
         <v>0.56899999999999995</v>
@@ -19214,7 +19268,7 @@
         <v>172</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>375</v>
+        <v>393</v>
       </c>
       <c r="D177">
         <v>0.57899999999999996</v>
@@ -19312,7 +19366,7 @@
         <v>173</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>378</v>
+        <v>396</v>
       </c>
       <c r="D178" t="s">
         <v>7</v>
@@ -19410,7 +19464,7 @@
         <v>174</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>371</v>
+        <v>389</v>
       </c>
       <c r="D179">
         <v>0.312</v>
@@ -19508,7 +19562,7 @@
         <v>175</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>370</v>
+        <v>388</v>
       </c>
       <c r="D180">
         <v>0.70499999999999996</v>
@@ -19606,7 +19660,7 @@
         <v>176</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>379</v>
+        <v>397</v>
       </c>
       <c r="D181">
         <v>0.72399999999999998</v>
@@ -19704,7 +19758,7 @@
         <v>177</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="D182">
         <v>0.77500000000000002</v>
@@ -19802,7 +19856,7 @@
         <v>178</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="D183">
         <v>0.86</v>
@@ -19900,7 +19954,7 @@
         <v>179</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
       <c r="D184">
         <v>0.69199999999999995</v>
@@ -19998,7 +20052,7 @@
         <v>180</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>376</v>
+        <v>394</v>
       </c>
       <c r="D185" t="s">
         <v>7</v>
@@ -20096,7 +20150,7 @@
         <v>181</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>372</v>
+        <v>390</v>
       </c>
       <c r="D186" t="s">
         <v>7</v>
@@ -20191,10 +20245,10 @@
         <v>96</v>
       </c>
       <c r="B187" t="s">
-        <v>381</v>
+        <v>399</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>373</v>
+        <v>391</v>
       </c>
       <c r="D187">
         <v>0.63800000000000001</v>
@@ -20292,7 +20346,7 @@
         <v>182</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>383</v>
+        <v>401</v>
       </c>
       <c r="D188">
         <v>0.47499999999999998</v>
@@ -20390,7 +20444,7 @@
         <v>183</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>382</v>
+        <v>400</v>
       </c>
       <c r="D189">
         <v>0.39200000000000002</v>
@@ -20488,7 +20542,7 @@
         <v>184</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>384</v>
+        <v>402</v>
       </c>
       <c r="D190">
         <v>0.42399999999999999</v>
@@ -20586,7 +20640,7 @@
         <v>185</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>385</v>
+        <v>403</v>
       </c>
       <c r="D191">
         <v>0.498</v>
@@ -20684,7 +20738,7 @@
         <v>186</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>386</v>
+        <v>404</v>
       </c>
       <c r="D192" t="s">
         <v>7</v>
@@ -20877,10 +20931,10 @@
         <v>7</v>
       </c>
       <c r="B194" t="s">
-        <v>387</v>
+        <v>405</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
       <c r="D194" t="s">
         <v>7</v>
@@ -20978,7 +21032,7 @@
         <v>188</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="D195" t="s">
         <v>7</v>
@@ -21076,7 +21130,7 @@
         <v>189</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>279</v>
+        <v>297</v>
       </c>
       <c r="D196" t="s">
         <v>7</v>
@@ -21174,7 +21228,7 @@
         <v>190</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
       <c r="D197" t="s">
         <v>7</v>
@@ -21262,6 +21316,1609 @@
       </c>
       <c r="AF197" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="198" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>191</v>
+      </c>
+      <c r="E198" t="s">
+        <v>7</v>
+      </c>
+      <c r="F198" t="s">
+        <v>7</v>
+      </c>
+      <c r="G198" t="s">
+        <v>7</v>
+      </c>
+      <c r="H198" t="s">
+        <v>7</v>
+      </c>
+      <c r="I198" t="s">
+        <v>7</v>
+      </c>
+      <c r="J198" t="s">
+        <v>7</v>
+      </c>
+      <c r="K198" t="s">
+        <v>7</v>
+      </c>
+      <c r="L198" t="s">
+        <v>7</v>
+      </c>
+      <c r="M198" t="s">
+        <v>7</v>
+      </c>
+      <c r="N198" t="s">
+        <v>7</v>
+      </c>
+      <c r="O198" t="s">
+        <v>7</v>
+      </c>
+      <c r="P198" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q198" t="s">
+        <v>7</v>
+      </c>
+      <c r="R198" t="s">
+        <v>7</v>
+      </c>
+      <c r="S198" t="s">
+        <v>7</v>
+      </c>
+      <c r="T198" t="s">
+        <v>7</v>
+      </c>
+      <c r="U198" t="s">
+        <v>7</v>
+      </c>
+      <c r="V198" t="s">
+        <v>7</v>
+      </c>
+      <c r="W198" t="s">
+        <v>7</v>
+      </c>
+      <c r="X198" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y198" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z198" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA198" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB198" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC198" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD198" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE198" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF198" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>192</v>
+      </c>
+      <c r="B199" t="s">
+        <v>193</v>
+      </c>
+      <c r="D199">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="E199">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="F199">
+        <v>0.78</v>
+      </c>
+      <c r="G199">
+        <v>0.79</v>
+      </c>
+      <c r="H199">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="I199">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="J199">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="K199">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="L199">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="M199">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="N199">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="O199">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="P199">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="Q199">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="R199">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="S199">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="T199">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="U199">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="V199">
+        <v>0.86</v>
+      </c>
+      <c r="W199">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="X199">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="Y199">
+        <v>0.871</v>
+      </c>
+      <c r="Z199">
+        <v>0.874</v>
+      </c>
+      <c r="AA199">
+        <v>0.878</v>
+      </c>
+      <c r="AB199">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="AC199">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="AD199">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="AE199">
+        <v>0.89</v>
+      </c>
+      <c r="AF199">
+        <v>0.89200000000000002</v>
+      </c>
+    </row>
+    <row r="200" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>192</v>
+      </c>
+      <c r="B200" t="s">
+        <v>194</v>
+      </c>
+      <c r="D200">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="E200">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="F200">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="G200">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="H200">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="I200">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="J200">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="K200">
+        <v>0.61</v>
+      </c>
+      <c r="L200">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="M200">
+        <v>0.622</v>
+      </c>
+      <c r="N200">
+        <v>0.63</v>
+      </c>
+      <c r="O200">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="P200">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="Q200">
+        <v>0.65</v>
+      </c>
+      <c r="R200">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="S200">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="T200">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="U200">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="V200">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="W200">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="X200">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="Y200">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="Z200">
+        <v>0.72</v>
+      </c>
+      <c r="AA200">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="AB200">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="AC200">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="AD200">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="AE200">
+        <v>0.746</v>
+      </c>
+      <c r="AF200">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="201" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>192</v>
+      </c>
+      <c r="B201" t="s">
+        <v>195</v>
+      </c>
+      <c r="D201">
+        <v>0.437</v>
+      </c>
+      <c r="E201">
+        <v>0.439</v>
+      </c>
+      <c r="F201">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="G201">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="H201">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="I201">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="J201">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="K201">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="L201">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="M201">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="N201">
+        <v>0.497</v>
+      </c>
+      <c r="O201">
+        <v>0.502</v>
+      </c>
+      <c r="P201">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="Q201">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="R201">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="S201">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="T201">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="U201">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="V201">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="W201">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="X201">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="Y201">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="Z201">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="AA201">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="AB201">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="AC201">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="AD201">
+        <v>0.625</v>
+      </c>
+      <c r="AE201">
+        <v>0.63</v>
+      </c>
+      <c r="AF201">
+        <v>0.63400000000000001</v>
+      </c>
+    </row>
+    <row r="202" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>192</v>
+      </c>
+      <c r="B202" t="s">
+        <v>196</v>
+      </c>
+      <c r="D202">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="E202">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="F202">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="G202">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="H202">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="I202">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="J202">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="K202">
+        <v>0.373</v>
+      </c>
+      <c r="L202">
+        <v>0.379</v>
+      </c>
+      <c r="M202">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="N202">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="O202">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="P202">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="Q202">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="R202">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="S202">
+        <v>0.435</v>
+      </c>
+      <c r="T202">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="U202">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="V202">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="W202">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="X202">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="Y202">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="Z202">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="AA202">
+        <v>0.49</v>
+      </c>
+      <c r="AB202">
+        <v>0.496</v>
+      </c>
+      <c r="AC202">
+        <v>0.499</v>
+      </c>
+      <c r="AD202">
+        <v>0.501</v>
+      </c>
+      <c r="AE202">
+        <v>0.505</v>
+      </c>
+      <c r="AF202">
+        <v>0.50700000000000001</v>
+      </c>
+    </row>
+    <row r="203" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>192</v>
+      </c>
+      <c r="B203" t="s">
+        <v>197</v>
+      </c>
+      <c r="D203">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="E203">
+        <v>0.52</v>
+      </c>
+      <c r="F203">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="G203">
+        <v>0.53</v>
+      </c>
+      <c r="H203">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="I203">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="J203">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="K203">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="L203">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="M203">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="N203">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="O203">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="P203">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="Q203">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="R203">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="S203">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="T203">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="U203">
+        <v>0.622</v>
+      </c>
+      <c r="V203">
+        <v>0.629</v>
+      </c>
+      <c r="W203">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="X203">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="Y203">
+        <v>0.65</v>
+      </c>
+      <c r="Z203">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="AA203">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="AB203">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="AC203">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="AD203">
+        <v>0.68</v>
+      </c>
+      <c r="AE203">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="AF203">
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="204" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
+        <v>198</v>
+      </c>
+      <c r="E204" t="s">
+        <v>7</v>
+      </c>
+      <c r="F204" t="s">
+        <v>7</v>
+      </c>
+      <c r="G204" t="s">
+        <v>7</v>
+      </c>
+      <c r="H204" t="s">
+        <v>7</v>
+      </c>
+      <c r="I204" t="s">
+        <v>7</v>
+      </c>
+      <c r="J204" t="s">
+        <v>7</v>
+      </c>
+      <c r="K204" t="s">
+        <v>7</v>
+      </c>
+      <c r="L204" t="s">
+        <v>7</v>
+      </c>
+      <c r="M204" t="s">
+        <v>7</v>
+      </c>
+      <c r="N204" t="s">
+        <v>7</v>
+      </c>
+      <c r="O204" t="s">
+        <v>7</v>
+      </c>
+      <c r="P204" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q204" t="s">
+        <v>7</v>
+      </c>
+      <c r="R204" t="s">
+        <v>7</v>
+      </c>
+      <c r="S204" t="s">
+        <v>7</v>
+      </c>
+      <c r="T204" t="s">
+        <v>7</v>
+      </c>
+      <c r="U204" t="s">
+        <v>7</v>
+      </c>
+      <c r="V204" t="s">
+        <v>7</v>
+      </c>
+      <c r="W204" t="s">
+        <v>7</v>
+      </c>
+      <c r="X204" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y204" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z204" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA204" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB204" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC204" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD204" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE204" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF204" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="205" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>192</v>
+      </c>
+      <c r="B205" t="s">
+        <v>199</v>
+      </c>
+      <c r="D205">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="E205">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="F205">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="G205">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="H205">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="I205">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="J205">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="K205">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="L205">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="M205">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="N205">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="O205">
+        <v>0.62</v>
+      </c>
+      <c r="P205">
+        <v>0.624</v>
+      </c>
+      <c r="Q205">
+        <v>0.63</v>
+      </c>
+      <c r="R205">
+        <v>0.64</v>
+      </c>
+      <c r="S205">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="T205">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="U205">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="V205">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="W205">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="X205">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="Y205">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="Z205">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="AA205">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="AB205">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="AC205">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="AD205">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="AE205">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="AF205">
+        <v>0.70299999999999996</v>
+      </c>
+    </row>
+    <row r="206" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>192</v>
+      </c>
+      <c r="B206" t="s">
+        <v>200</v>
+      </c>
+      <c r="D206">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="E206">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="F206">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="G206">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="H206">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="I206">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="J206">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="K206">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="L206">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="M206">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="N206">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="O206">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="P206">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="Q206">
+        <v>0.623</v>
+      </c>
+      <c r="R206">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="S206">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="T206">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="U206">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="V206">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="W206">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="X206">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="Y206">
+        <v>0.7</v>
+      </c>
+      <c r="Z206">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="AA206">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="AB206">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="AC206">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="AD206">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="AE206">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="AF206">
+        <v>0.74099999999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>192</v>
+      </c>
+      <c r="B207" t="s">
+        <v>201</v>
+      </c>
+      <c r="D207">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="E207">
+        <v>0.65</v>
+      </c>
+      <c r="F207">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="G207">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="H207">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="I207">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="J207">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="K207">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="L207">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="M207">
+        <v>0.66</v>
+      </c>
+      <c r="N207">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="O207">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="P207">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="Q207">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="R207">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="S207">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="T207">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="U207">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="V207">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="W207">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="X207">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="Y207">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="Z207">
+        <v>0.75</v>
+      </c>
+      <c r="AA207">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="AB207">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="AC207">
+        <v>0.77</v>
+      </c>
+      <c r="AD207">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="AE207">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="AF207">
+        <v>0.77900000000000003</v>
+      </c>
+    </row>
+    <row r="208" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>192</v>
+      </c>
+      <c r="B208" t="s">
+        <v>202</v>
+      </c>
+      <c r="D208">
+        <v>0.628</v>
+      </c>
+      <c r="E208">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="F208">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="G208">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="H208">
+        <v>0.65</v>
+      </c>
+      <c r="I208">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="J208">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="K208">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="L208">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="M208">
+        <v>0.68</v>
+      </c>
+      <c r="N208">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="O208">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="P208">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="Q208">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="R208">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="S208">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="T208">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="U208">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="V208">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="W208">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="X208">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="Y208">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="Z208">
+        <v>0.74</v>
+      </c>
+      <c r="AA208">
+        <v>0.748</v>
+      </c>
+      <c r="AB208">
+        <v>0.752</v>
+      </c>
+      <c r="AC208">
+        <v>0.754</v>
+      </c>
+      <c r="AD208">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="AE208">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="AF208">
+        <v>0.75900000000000001</v>
+      </c>
+    </row>
+    <row r="209" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>192</v>
+      </c>
+      <c r="B209" t="s">
+        <v>203</v>
+      </c>
+      <c r="D209">
+        <v>0.441</v>
+      </c>
+      <c r="E209">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="F209">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="G209">
+        <v>0.46</v>
+      </c>
+      <c r="H209">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="I209">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="J209">
+        <v>0.48</v>
+      </c>
+      <c r="K209">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="L209">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="M209">
+        <v>0.499</v>
+      </c>
+      <c r="N209">
+        <v>0.505</v>
+      </c>
+      <c r="O209">
+        <v>0.51</v>
+      </c>
+      <c r="P209">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="Q209">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="R209">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="S209">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="T209">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="U209">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="V209">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="W209">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="X209">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="Y209">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="Z209">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="AA209">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="AB209">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="AC209">
+        <v>0.624</v>
+      </c>
+      <c r="AD209">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="AE209">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="AF209">
+        <v>0.64200000000000002</v>
+      </c>
+    </row>
+    <row r="210" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>192</v>
+      </c>
+      <c r="B210" t="s">
+        <v>204</v>
+      </c>
+      <c r="D210">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="E210">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="F210">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="G210">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="H210">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="I210">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="J210">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="K210">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="L210">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="M210">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="N210">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="O210">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="P210">
+        <v>0.434</v>
+      </c>
+      <c r="Q210">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="R210">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="S210">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="T210">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="U210">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="V210">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="W210">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="X210">
+        <v>0.498</v>
+      </c>
+      <c r="Y210">
+        <v>0.505</v>
+      </c>
+      <c r="Z210">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="AA210">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="AB210">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="AC210">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="AD210">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="AE210">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="AF210">
+        <v>0.54100000000000004</v>
+      </c>
+    </row>
+    <row r="211" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>192</v>
+      </c>
+      <c r="B211" t="s">
+        <v>205</v>
+      </c>
+      <c r="D211">
+        <v>0.35</v>
+      </c>
+      <c r="E211">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="F211">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="G211">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="H211">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="I211">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="J211">
+        <v>0.374</v>
+      </c>
+      <c r="K211">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="L211">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="M211">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="N211">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="O211">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="P211">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="Q211">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="R211">
+        <v>0.43</v>
+      </c>
+      <c r="S211">
+        <v>0.439</v>
+      </c>
+      <c r="T211">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="U211">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="V211">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="W211">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="X211">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="Y211">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="Z211">
+        <v>0.499</v>
+      </c>
+      <c r="AA211">
+        <v>0.504</v>
+      </c>
+      <c r="AB211">
+        <v>0.51</v>
+      </c>
+      <c r="AC211">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="AD211">
+        <v>0.52</v>
+      </c>
+      <c r="AE211">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="AF211">
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="212" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>192</v>
+      </c>
+      <c r="B212" t="s">
+        <v>206</v>
+      </c>
+      <c r="D212">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="E212">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="F212">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="G212">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="H212">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="I212">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="J212">
+        <v>0.624</v>
+      </c>
+      <c r="K212">
+        <v>0.629</v>
+      </c>
+      <c r="L212">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="M212">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="N212">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="O212">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="P212">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="Q212">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="R212">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="S212">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="T212">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="U212">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="V212">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="W212">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="X212">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="Y212">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="Z212">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="AA212">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="AB212">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="AC212">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="AD212">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="AE212">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="AF212">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="213" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>192</v>
+      </c>
+      <c r="B213" t="s">
+        <v>207</v>
+      </c>
+      <c r="D213">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="E213">
+        <v>0.79</v>
+      </c>
+      <c r="F213">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="G213">
+        <v>0.8</v>
+      </c>
+      <c r="H213">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="I213">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="J213">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="K213">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="L213">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="M213">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="N213">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="O213">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="P213">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="Q213">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="R213">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="S213">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="T213">
+        <v>0.86</v>
+      </c>
+      <c r="U213">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="V213">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="W213">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="X213">
+        <v>0.873</v>
+      </c>
+      <c r="Y213">
+        <v>0.877</v>
+      </c>
+      <c r="Z213">
+        <v>0.879</v>
+      </c>
+      <c r="AA213">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="AB213">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="AC213">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="AD213">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="AE213">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="AF213">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="214" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>192</v>
+      </c>
+      <c r="B214" t="s">
+        <v>208</v>
+      </c>
+      <c r="D214">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="E214">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="F214">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="G214">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="H214">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="I214">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="J214">
+        <v>0.622</v>
+      </c>
+      <c r="K214">
+        <v>0.624</v>
+      </c>
+      <c r="L214">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="M214">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="N214">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="O214">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="P214">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="Q214">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="R214">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="S214">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="T214">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="U214">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="V214">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="W214">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="X214">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="Y214">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="Z214">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="AA214">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="AB214">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="AC214">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="AD214">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="AE214">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="AF214">
+        <v>0.73099999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>